<commit_message>
SBI-422: Prepare ArkCase priority list to be able to be overrided by Bactes360
</commit_message>
<xml_diff>
--- a/acm-plugins/acm-default-plugins/acm-case-file-plugin/src/main/resources/rules/Bactes360/drools-case-file-rules.xlsx
+++ b/acm-plugins/acm-default-plugins/acm-case-file-plugin/src/main/resources/rules/Bactes360/drools-case-file-rules.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manoj.dhungana\.acm\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riste.tutureski\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -168,9 +168,6 @@
     <t>priority == null</t>
   </si>
   <si>
-    <t>setPriority,'Medium'</t>
-  </si>
-  <si>
     <t>Set Due Date</t>
   </si>
   <si>
@@ -187,6 +184,9 @@
   </si>
   <si>
     <t>setTitle, dateFormat('yyyyMMdd') + '_' + $caseFile.getId()</t>
+  </si>
+  <si>
+    <t>setPriority,'Normal'</t>
   </si>
 </sst>
 </file>
@@ -825,8 +825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1074,31 +1074,31 @@
         <v>38</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="D26" s="17" t="s">
         <v>41</v>
-      </c>
-      <c r="D26" s="17" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="C27" s="17" t="s">
+      <c r="D27" s="17" t="s">
         <v>44</v>
-      </c>
-      <c r="D27" s="17" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>